<commit_message>
adds camera data adds script analyzing flowering time patterns
</commit_message>
<xml_diff>
--- a/data/raw/opening_camera_2025.xlsx
+++ b/data/raw/opening_camera_2025.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10309"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10315"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/gretchen/GitHub/CApoppy/data/raw/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5AAF0130-CD42-144A-B183-3E35971A4439}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6D8A425B-C408-494C-BE77-D1CF24D2C7C2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="18620" yWindow="2420" windowWidth="32460" windowHeight="21520" xr2:uid="{ADDEA5CE-D739-0A42-9E9A-291E5DFE88D1}"/>
+    <workbookView xWindow="12220" yWindow="19320" windowWidth="32460" windowHeight="21520" xr2:uid="{ADDEA5CE-D739-0A42-9E9A-291E5DFE88D1}"/>
   </bookViews>
   <sheets>
     <sheet name="data" sheetId="1" r:id="rId1"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="64" uniqueCount="32">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="92" uniqueCount="39">
   <si>
     <t>Locality</t>
   </si>
@@ -133,6 +133,27 @@
   </si>
   <si>
     <t>before 9:20</t>
+  </si>
+  <si>
+    <t>before 8:14</t>
+  </si>
+  <si>
+    <t>new flower</t>
+  </si>
+  <si>
+    <t>1st petal abscises</t>
+  </si>
+  <si>
+    <t>Time available</t>
+  </si>
+  <si>
+    <t>NA</t>
+  </si>
+  <si>
+    <t>1st petal abcises</t>
+  </si>
+  <si>
+    <t>15;40</t>
   </si>
 </sst>
 </file>
@@ -506,10 +527,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B46123D7-FB67-C94C-8A63-35CDF23A6312}">
-  <dimension ref="A1:R16"/>
+  <dimension ref="A1:S26"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D31" sqref="D31"/>
+      <pane ySplit="1" topLeftCell="A17" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="P23" sqref="P23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -518,7 +540,7 @@
     <col min="15" max="15" width="18.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -573,8 +595,11 @@
       <c r="R1" t="s">
         <v>16</v>
       </c>
-    </row>
-    <row r="2" spans="1:18" x14ac:dyDescent="0.2">
+      <c r="S1" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="2" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>18</v>
       </c>
@@ -624,7 +649,7 @@
         <v>0.11805555555555552</v>
       </c>
     </row>
-    <row r="3" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>18</v>
       </c>
@@ -674,7 +699,7 @@
         <v>7.6388888888888951E-2</v>
       </c>
     </row>
-    <row r="4" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>18</v>
       </c>
@@ -721,7 +746,7 @@
         <v>0.15972222222222227</v>
       </c>
     </row>
-    <row r="5" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>18</v>
       </c>
@@ -743,7 +768,7 @@
       <c r="P5" s="2"/>
       <c r="Q5" s="2"/>
     </row>
-    <row r="6" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>13</v>
       </c>
@@ -772,7 +797,7 @@
       </c>
       <c r="R6" s="2"/>
     </row>
-    <row r="7" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>13</v>
       </c>
@@ -804,7 +829,7 @@
         <v>4.166666666666663E-2</v>
       </c>
     </row>
-    <row r="8" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
         <v>13</v>
       </c>
@@ -826,13 +851,16 @@
       <c r="P8" s="2"/>
       <c r="Q8" s="2"/>
     </row>
-    <row r="9" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
         <v>18</v>
       </c>
       <c r="B9">
         <v>8</v>
       </c>
+      <c r="C9" s="1">
+        <v>45727</v>
+      </c>
       <c r="D9" t="s">
         <v>31</v>
       </c>
@@ -846,10 +874,16 @@
         <v>0.61111111111111116</v>
       </c>
     </row>
-    <row r="10" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:19" x14ac:dyDescent="0.2">
+      <c r="A10" t="s">
+        <v>18</v>
+      </c>
       <c r="B10">
         <v>8</v>
       </c>
+      <c r="C10" s="1">
+        <v>45727</v>
+      </c>
       <c r="D10" t="s">
         <v>31</v>
       </c>
@@ -860,10 +894,16 @@
         <v>3948</v>
       </c>
     </row>
-    <row r="11" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:19" x14ac:dyDescent="0.2">
+      <c r="A11" t="s">
+        <v>18</v>
+      </c>
       <c r="B11">
         <v>9</v>
       </c>
+      <c r="C11" s="1">
+        <v>45727</v>
+      </c>
       <c r="D11" t="s">
         <v>31</v>
       </c>
@@ -874,10 +914,16 @@
         <v>3944</v>
       </c>
     </row>
-    <row r="12" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:19" x14ac:dyDescent="0.2">
+      <c r="A12" t="s">
+        <v>18</v>
+      </c>
       <c r="B12">
         <v>10</v>
       </c>
+      <c r="C12" s="1">
+        <v>45727</v>
+      </c>
       <c r="D12" t="s">
         <v>31</v>
       </c>
@@ -888,10 +934,16 @@
         <v>3948</v>
       </c>
     </row>
-    <row r="13" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:19" x14ac:dyDescent="0.2">
+      <c r="A13" t="s">
+        <v>18</v>
+      </c>
       <c r="B13">
         <v>11</v>
       </c>
+      <c r="C13" s="1">
+        <v>45727</v>
+      </c>
       <c r="D13" t="s">
         <v>31</v>
       </c>
@@ -902,10 +954,16 @@
         <v>3948</v>
       </c>
     </row>
-    <row r="14" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:19" x14ac:dyDescent="0.2">
+      <c r="A14" t="s">
+        <v>18</v>
+      </c>
       <c r="B14">
         <v>12</v>
       </c>
+      <c r="C14" s="1">
+        <v>45727</v>
+      </c>
       <c r="D14" t="s">
         <v>31</v>
       </c>
@@ -916,10 +974,16 @@
         <v>3944</v>
       </c>
     </row>
-    <row r="15" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:19" x14ac:dyDescent="0.2">
+      <c r="A15" t="s">
+        <v>18</v>
+      </c>
       <c r="B15">
         <v>13</v>
       </c>
+      <c r="C15" s="1">
+        <v>45727</v>
+      </c>
       <c r="D15" t="s">
         <v>31</v>
       </c>
@@ -930,10 +994,16 @@
         <v>3954</v>
       </c>
     </row>
-    <row r="16" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:19" x14ac:dyDescent="0.2">
+      <c r="A16" t="s">
+        <v>18</v>
+      </c>
       <c r="B16">
         <v>13</v>
       </c>
+      <c r="C16" s="1">
+        <v>45727</v>
+      </c>
       <c r="D16" s="2">
         <v>0.3888888888888889</v>
       </c>
@@ -945,6 +1015,330 @@
       </c>
       <c r="K16" t="s">
         <v>11</v>
+      </c>
+    </row>
+    <row r="17" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A17" t="s">
+        <v>13</v>
+      </c>
+      <c r="B17">
+        <v>14</v>
+      </c>
+      <c r="C17" s="1">
+        <v>45731</v>
+      </c>
+      <c r="D17" t="s">
+        <v>32</v>
+      </c>
+      <c r="G17" s="2">
+        <v>0.40555555555555556</v>
+      </c>
+      <c r="H17">
+        <v>6303</v>
+      </c>
+      <c r="J17" s="2">
+        <v>0.55138888888888893</v>
+      </c>
+      <c r="K17">
+        <v>6324</v>
+      </c>
+      <c r="L17" t="s">
+        <v>34</v>
+      </c>
+      <c r="M17" s="2"/>
+    </row>
+    <row r="18" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A18" t="s">
+        <v>13</v>
+      </c>
+      <c r="B18">
+        <v>15</v>
+      </c>
+      <c r="C18" s="1">
+        <v>45731</v>
+      </c>
+      <c r="D18" s="2">
+        <v>0.45416666666666666</v>
+      </c>
+      <c r="E18">
+        <v>6310</v>
+      </c>
+      <c r="G18" s="2">
+        <v>0.53055555555555556</v>
+      </c>
+      <c r="H18">
+        <v>6321</v>
+      </c>
+      <c r="J18" s="2">
+        <v>0.67638888888888893</v>
+      </c>
+      <c r="K18">
+        <v>6342</v>
+      </c>
+      <c r="M18" s="2">
+        <v>0.77361111111111114</v>
+      </c>
+      <c r="N18">
+        <v>6356</v>
+      </c>
+    </row>
+    <row r="19" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A19" t="s">
+        <v>13</v>
+      </c>
+      <c r="B19">
+        <v>16</v>
+      </c>
+      <c r="C19" s="1">
+        <v>45731</v>
+      </c>
+      <c r="D19" s="2">
+        <v>0.46805555555555556</v>
+      </c>
+      <c r="F19" t="s">
+        <v>33</v>
+      </c>
+      <c r="G19" s="2">
+        <v>0.53055555555555556</v>
+      </c>
+      <c r="H19">
+        <v>6321</v>
+      </c>
+      <c r="J19" s="2">
+        <v>0.63472222222222219</v>
+      </c>
+      <c r="K19">
+        <v>6336</v>
+      </c>
+      <c r="M19" s="2">
+        <v>0.73888888888888893</v>
+      </c>
+      <c r="N19">
+        <v>6351</v>
+      </c>
+    </row>
+    <row r="20" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A20" t="s">
+        <v>13</v>
+      </c>
+      <c r="B20">
+        <v>15</v>
+      </c>
+      <c r="C20" s="1">
+        <v>45732</v>
+      </c>
+      <c r="D20" t="s">
+        <v>36</v>
+      </c>
+      <c r="G20" t="s">
+        <v>36</v>
+      </c>
+      <c r="J20" s="2">
+        <v>0.69027777777777777</v>
+      </c>
+      <c r="K20">
+        <v>6434</v>
+      </c>
+      <c r="M20" s="2">
+        <v>0.73888888888888893</v>
+      </c>
+      <c r="N20">
+        <v>6441</v>
+      </c>
+    </row>
+    <row r="21" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A21" t="s">
+        <v>13</v>
+      </c>
+      <c r="B21">
+        <v>16</v>
+      </c>
+      <c r="C21" s="1">
+        <v>45732</v>
+      </c>
+      <c r="D21" t="s">
+        <v>36</v>
+      </c>
+      <c r="G21" t="s">
+        <v>36</v>
+      </c>
+      <c r="J21" s="2">
+        <v>0.64861111111111114</v>
+      </c>
+      <c r="K21">
+        <v>6428</v>
+      </c>
+      <c r="M21" s="2">
+        <v>0.71111111111111114</v>
+      </c>
+      <c r="N21">
+        <v>6437</v>
+      </c>
+    </row>
+    <row r="22" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A22" t="s">
+        <v>13</v>
+      </c>
+      <c r="B22">
+        <v>17</v>
+      </c>
+      <c r="C22" s="1">
+        <v>45732</v>
+      </c>
+      <c r="D22" s="2">
+        <v>0.35416666666666669</v>
+      </c>
+      <c r="E22">
+        <v>4133</v>
+      </c>
+    </row>
+    <row r="23" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A23" t="s">
+        <v>13</v>
+      </c>
+      <c r="B23">
+        <v>18</v>
+      </c>
+      <c r="C23" s="1">
+        <v>45731</v>
+      </c>
+      <c r="D23" s="2">
+        <v>0.3611111111111111</v>
+      </c>
+      <c r="E23">
+        <v>3991</v>
+      </c>
+      <c r="G23" s="2">
+        <v>0.4236111111111111</v>
+      </c>
+      <c r="H23">
+        <v>4000</v>
+      </c>
+      <c r="J23" s="2">
+        <v>0.63888888888888884</v>
+      </c>
+      <c r="K23">
+        <v>4031</v>
+      </c>
+      <c r="L23" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="24" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A24" t="s">
+        <v>13</v>
+      </c>
+      <c r="B24">
+        <v>19</v>
+      </c>
+      <c r="C24" s="1">
+        <v>45731</v>
+      </c>
+      <c r="D24" s="2">
+        <v>0.375</v>
+      </c>
+      <c r="E24">
+        <v>3993</v>
+      </c>
+      <c r="G24" s="2">
+        <v>0.47916666666666669</v>
+      </c>
+      <c r="H24">
+        <v>4008</v>
+      </c>
+      <c r="J24" s="2">
+        <v>0.66666666666666663</v>
+      </c>
+      <c r="K24">
+        <v>4035</v>
+      </c>
+      <c r="L24" s="2">
+        <v>0.70833333333333337</v>
+      </c>
+      <c r="M24" s="2">
+        <v>0.70833333333333337</v>
+      </c>
+      <c r="N24" s="2">
+        <v>4041</v>
+      </c>
+    </row>
+    <row r="25" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A25" t="s">
+        <v>13</v>
+      </c>
+      <c r="B25">
+        <v>20</v>
+      </c>
+      <c r="C25" s="1">
+        <v>45731</v>
+      </c>
+      <c r="D25" s="2">
+        <v>0.41666666666666669</v>
+      </c>
+      <c r="E25">
+        <v>3999</v>
+      </c>
+      <c r="G25" s="2">
+        <v>0.54861111111111116</v>
+      </c>
+      <c r="H25">
+        <v>4016</v>
+      </c>
+      <c r="J25" t="s">
+        <v>38</v>
+      </c>
+      <c r="K25">
+        <v>4033</v>
+      </c>
+      <c r="L25" s="2">
+        <v>0.70138888888888884</v>
+      </c>
+      <c r="M25" s="2">
+        <v>0.70138888888888884</v>
+      </c>
+      <c r="N25">
+        <v>4040</v>
+      </c>
+    </row>
+    <row r="26" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A26" t="s">
+        <v>13</v>
+      </c>
+      <c r="B26">
+        <v>21</v>
+      </c>
+      <c r="C26" s="1">
+        <v>45731</v>
+      </c>
+      <c r="D26" s="2">
+        <v>0.41666666666666669</v>
+      </c>
+      <c r="E26">
+        <v>3999</v>
+      </c>
+      <c r="F26" t="s">
+        <v>33</v>
+      </c>
+      <c r="G26" s="2">
+        <v>0.54166666666666663</v>
+      </c>
+      <c r="H26">
+        <v>4017</v>
+      </c>
+      <c r="J26" s="2">
+        <v>0.63888888888888884</v>
+      </c>
+      <c r="K26">
+        <v>4031</v>
+      </c>
+      <c r="L26" s="2">
+        <v>0.71527777777777779</v>
+      </c>
+      <c r="M26" s="2">
+        <v>0.71527777777777779</v>
+      </c>
+      <c r="N26">
+        <v>4042</v>
       </c>
     </row>
   </sheetData>

</xml_diff>